<commit_message>
copiati nuove soluzioni. ora disegnare frontiera
</commit_message>
<xml_diff>
--- a/logs/benchmarks.xlsx
+++ b/logs/benchmarks.xlsx
@@ -64,13 +64,13 @@
     <t>ALG</t>
   </si>
   <si>
-    <t>?????????</t>
-  </si>
-  <si>
     <t>4 threads su 2 cores in hyperthreading</t>
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>Automatic</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="11">
         <v>5.4179127999999998E-4</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="11">
         <v>5.4179127999999998E-4</v>

</xml_diff>